<commit_message>
25.07 баги в extract и transform
</commit_message>
<xml_diff>
--- a/data_input/analytics/Agents GPU.xlsx
+++ b/data_input/analytics/Agents GPU.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="71">
   <si>
     <t>Эксплуатация</t>
   </si>
@@ -979,9 +979,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -989,40 +989,41 @@
     <col min="1" max="1" width="24" style="6" customWidth="1"/>
     <col min="2" max="2" width="15.7265625" style="6" customWidth="1"/>
     <col min="3" max="3" width="14" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14" style="13" customWidth="1"/>
-    <col min="6" max="6" width="23.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="13" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.1796875" style="18" customWidth="1"/>
     <col min="10" max="10" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.36328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.453125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="28.1796875" style="18" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7265625" style="18" customWidth="1"/>
     <col min="14" max="14" width="8.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.36328125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.453125" style="19" customWidth="1"/>
+    <col min="16" max="16" width="10.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="22.453125" style="19" customWidth="1"/>
     <col min="18" max="18" width="9.54296875" style="1" customWidth="1"/>
     <col min="19" max="19" width="15.08984375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.26953125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.26953125" style="1" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.453125" style="1" customWidth="1"/>
     <col min="23" max="23" width="19.54296875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="23.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.90625" style="19" customWidth="1"/>
     <col min="25" max="25" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="17.81640625" style="18" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="14.54296875" style="1" customWidth="1"/>
-    <col min="31" max="31" width="9.54296875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="16.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.81640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.1796875" style="1" customWidth="1"/>
-    <col min="38" max="39" width="19.453125" style="18" customWidth="1"/>
+    <col min="31" max="31" width="9.54296875" style="1" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="16.453125" style="20" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="9" style="1" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="12.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="17.81640625" style="20" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="9" style="1" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="9.1796875" style="1" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="19.453125" style="18" customWidth="1"/>
+    <col min="39" max="39" width="16.453125" style="18" customWidth="1"/>
     <col min="40" max="40" width="28.1796875" style="1" customWidth="1"/>
     <col min="41" max="41" width="17.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="15.90625" style="1" bestFit="1" customWidth="1"/>
@@ -1283,9 +1284,7 @@
       <c r="AK2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AL2" s="10" t="s">
-        <v>62</v>
-      </c>
+      <c r="AL2" s="10"/>
       <c r="AM2" s="9" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
28.07 MacroProperty1 и md_components с проблемами
</commit_message>
<xml_diff>
--- a/data_input/analytics/Agents GPU.xlsx
+++ b/data_input/analytics/Agents GPU.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885E02B5-1F3B-4BF1-BC7D-C70FD5C7918F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="587"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="587" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Агенты" sheetId="4" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="72">
   <si>
     <t>Эксплуатация</t>
   </si>
@@ -307,13 +308,16 @@
   <si>
     <t>Macroproperty3 + PostProcessing - планеры</t>
   </si>
+  <si>
+    <t>psn</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;\ _₽_-;_-@_-"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -623,22 +627,22 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="19" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -662,7 +666,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -674,8 +678,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1"/>
-    <cellStyle name="Обычный 3" xfId="2"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -766,6 +770,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -801,6 +822,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -976,69 +1014,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL2" sqref="AL2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="14" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="13" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1796875" style="18" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.36328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.453125" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7265625" style="18" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.36328125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="10.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="22.453125" style="19" customWidth="1"/>
-    <col min="18" max="18" width="9.54296875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15.08984375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.453125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="19.54296875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="15.90625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="18" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="18" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="22.42578125" style="19" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="15.85546875" style="19" customWidth="1"/>
     <col min="25" max="25" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.81640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.54296875" style="1" customWidth="1"/>
-    <col min="31" max="31" width="9.54296875" style="1" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="16.453125" style="20" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="9.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="16.42578125" style="20" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="9" style="1" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="12.26953125" style="1" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="17.81640625" style="20" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="17.85546875" style="20" hidden="1" customWidth="1"/>
     <col min="36" max="36" width="9" style="1" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="9.1796875" style="1" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="19.453125" style="18" customWidth="1"/>
-    <col min="39" max="39" width="16.453125" style="18" customWidth="1"/>
-    <col min="40" max="40" width="28.1796875" style="1" customWidth="1"/>
-    <col min="41" max="41" width="17.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="17.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="17.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="19.42578125" style="18" customWidth="1"/>
+    <col min="39" max="39" width="16.42578125" style="18" customWidth="1"/>
+    <col min="40" max="40" width="28.140625" style="1" customWidth="1"/>
+    <col min="41" max="41" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="16384" width="8.453125" style="1"/>
+    <col min="49" max="49" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="16384" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -1188,7 +1226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:50" s="6" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:50" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>68</v>
       </c>
@@ -1322,7 +1360,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:50" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>69</v>
       </c>
@@ -1331,7 +1369,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>21</v>
@@ -1472,7 +1510,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:50" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>34</v>
       </c>
@@ -1536,7 +1574,7 @@
       <c r="AW4" s="40"/>
       <c r="AX4" s="40"/>
     </row>
-    <row r="5" spans="1:50" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:50" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
@@ -1622,7 +1660,7 @@
       <c r="AW5" s="40"/>
       <c r="AX5" s="40"/>
     </row>
-    <row r="6" spans="1:50" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:50" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1714,7 +1752,7 @@
       <c r="AW6" s="40"/>
       <c r="AX6" s="40"/>
     </row>
-    <row r="7" spans="1:50" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:50" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1820,7 +1858,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
@@ -1886,7 +1924,7 @@
       <c r="AW8" s="40"/>
       <c r="AX8" s="40"/>
     </row>
-    <row r="9" spans="1:50" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:50" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -1968,7 +2006,7 @@
       <c r="AW9" s="40"/>
       <c r="AX9" s="40"/>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
@@ -2026,98 +2064,98 @@
       <c r="AW10" s="40"/>
       <c r="AX10" s="40"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="AN11" s="2"/>
       <c r="AO11" s="2"/>
       <c r="AP11" s="2"/>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="2"/>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="2"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="AN15" s="2"/>
       <c r="AO15" s="46"/>
       <c r="AP15" s="46"/>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="46"/>
       <c r="AP16" s="46"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AN17" s="2"/>
       <c r="AO17" s="46"/>
       <c r="AP17" s="46"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AN18" s="2"/>
       <c r="AO18" s="46"/>
       <c r="AP18" s="46"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
       <c r="AP19" s="2"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AN25" s="3"/>
       <c r="AO25" s="3"/>
       <c r="AP25" s="3"/>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AN26" s="4"/>
       <c r="AO26" s="4"/>
       <c r="AP26" s="4"/>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AN27" s="4"/>
       <c r="AO27" s="4"/>
       <c r="AP27" s="4"/>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AN28" s="4"/>
       <c r="AO28" s="4"/>
       <c r="AP28" s="4"/>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AN29" s="4"/>
       <c r="AO29" s="4"/>
       <c r="AP29" s="4"/>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AN30" s="4"/>
       <c r="AO30" s="4"/>
       <c r="AP30" s="4"/>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AN31" s="4"/>
       <c r="AO31" s="4"/>
       <c r="AP31" s="4"/>

</xml_diff>